<commit_message>
this took way too long
</commit_message>
<xml_diff>
--- a/Lab 6/data/Exp2.xlsx
+++ b/Lab 6/data/Exp2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Firelovesnow\Documents\PHYS-258\Lab 6\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Home\Desktop\School\20189-W-McGill\PHYS258\phys-258-coding\Lab 6\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0F342F-D832-4F8B-A3FF-9A162E1B3DD8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="3240" windowWidth="28800" windowHeight="10725" xr2:uid="{77094CF2-0E74-498F-B340-42A5960A8C78}"/>
+    <workbookView xWindow="3180" yWindow="3240" windowWidth="28800" windowHeight="10728"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,14 +383,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4FE2B2-BC39-4B83-9893-7B3844D541C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,7 +410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -431,7 +430,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>4</v>
       </c>
@@ -451,7 +450,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>6</v>
       </c>
@@ -471,7 +470,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8</v>
       </c>
@@ -491,7 +490,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>10</v>
       </c>
@@ -511,7 +510,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>12</v>
       </c>
@@ -531,7 +530,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>14</v>
       </c>
@@ -551,7 +550,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>16</v>
       </c>
@@ -571,7 +570,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>18</v>
       </c>
@@ -591,7 +590,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>20</v>
       </c>
@@ -611,7 +610,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>22</v>
       </c>
@@ -631,7 +630,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>24</v>
       </c>
@@ -651,7 +650,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>26</v>
       </c>
@@ -671,7 +670,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>28</v>
       </c>
@@ -691,7 +690,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>30</v>
       </c>
@@ -711,7 +710,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>32</v>
       </c>
@@ -731,7 +730,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>34</v>
       </c>
@@ -751,7 +750,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>36</v>
       </c>
@@ -771,7 +770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>38</v>
       </c>
@@ -791,7 +790,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>40</v>
       </c>
@@ -811,7 +810,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>42</v>
       </c>
@@ -831,7 +830,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>44</v>
       </c>
@@ -851,7 +850,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>46</v>
       </c>
@@ -871,7 +870,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>48</v>
       </c>
@@ -891,7 +890,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>50</v>
       </c>
@@ -911,7 +910,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>52</v>
       </c>
@@ -931,7 +930,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>54</v>
       </c>
@@ -951,7 +950,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>56</v>
       </c>
@@ -971,7 +970,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>58</v>
       </c>
@@ -991,7 +990,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>60</v>
       </c>
@@ -1011,7 +1010,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>62</v>
       </c>
@@ -1031,7 +1030,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>64</v>
       </c>
@@ -1051,7 +1050,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>66</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>68</v>
       </c>
@@ -1091,7 +1090,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>70</v>
       </c>
@@ -1111,7 +1110,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>72</v>
       </c>
@@ -1131,7 +1130,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>74</v>
       </c>
@@ -1151,7 +1150,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>76</v>
       </c>
@@ -1171,7 +1170,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>78</v>
       </c>
@@ -1191,7 +1190,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>80</v>
       </c>
@@ -1211,7 +1210,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>82</v>
       </c>
@@ -1231,7 +1230,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>84</v>
       </c>
@@ -1251,7 +1250,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>86</v>
       </c>
@@ -1271,7 +1270,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>88</v>
       </c>
@@ -1291,7 +1290,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>90</v>
       </c>
@@ -1311,7 +1310,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>92</v>
       </c>
@@ -1331,7 +1330,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>94</v>
       </c>
@@ -1351,7 +1350,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>96</v>
       </c>
@@ -1371,7 +1370,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>98</v>
       </c>
@@ -1391,7 +1390,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>100</v>
       </c>
@@ -1411,7 +1410,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>102</v>
       </c>
@@ -1431,7 +1430,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>104</v>
       </c>
@@ -1451,7 +1450,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>106</v>
       </c>
@@ -1471,7 +1470,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>108</v>
       </c>
@@ -1491,7 +1490,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>110</v>
       </c>
@@ -1511,7 +1510,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>112</v>
       </c>
@@ -1531,7 +1530,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>114</v>
       </c>
@@ -1551,7 +1550,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>116</v>
       </c>
@@ -1571,7 +1570,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>118</v>
       </c>
@@ -1591,7 +1590,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>120</v>
       </c>
@@ -1611,7 +1610,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>122</v>
       </c>
@@ -1631,7 +1630,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>124</v>
       </c>
@@ -1651,7 +1650,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>126</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>128</v>
       </c>
@@ -1691,7 +1690,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>130</v>
       </c>
@@ -1711,7 +1710,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>132</v>
       </c>
@@ -1731,7 +1730,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>134</v>
       </c>
@@ -1751,7 +1750,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>136</v>
       </c>
@@ -1771,7 +1770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>138</v>
       </c>
@@ -1791,7 +1790,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>140</v>
       </c>
@@ -1811,7 +1810,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>142</v>
       </c>
@@ -1831,7 +1830,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>144</v>
       </c>
@@ -1851,7 +1850,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>146</v>
       </c>
@@ -1871,7 +1870,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>148</v>
       </c>
@@ -1891,7 +1890,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>150</v>
       </c>
@@ -1911,7 +1910,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>152</v>
       </c>
@@ -1931,7 +1930,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>154</v>
       </c>
@@ -1951,7 +1950,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>156</v>
       </c>
@@ -1971,7 +1970,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>158</v>
       </c>
@@ -1991,7 +1990,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>160</v>
       </c>
@@ -2011,7 +2010,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>162</v>
       </c>
@@ -2031,7 +2030,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>164</v>
       </c>
@@ -2051,7 +2050,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>166</v>
       </c>
@@ -2071,7 +2070,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>168</v>
       </c>
@@ -2091,7 +2090,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>170</v>
       </c>
@@ -2111,7 +2110,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>172</v>
       </c>
@@ -2131,7 +2130,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>174</v>
       </c>
@@ -2151,7 +2150,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>176</v>
       </c>
@@ -2171,7 +2170,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>178</v>
       </c>
@@ -2191,7 +2190,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>180</v>
       </c>
@@ -2211,7 +2210,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>182</v>
       </c>
@@ -2231,7 +2230,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>184</v>
       </c>
@@ -2251,7 +2250,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>186</v>
       </c>
@@ -2271,7 +2270,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>188</v>
       </c>
@@ -2291,7 +2290,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>190</v>
       </c>
@@ -2311,7 +2310,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>192</v>
       </c>
@@ -2331,7 +2330,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>194</v>
       </c>
@@ -2351,7 +2350,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>196</v>
       </c>
@@ -2371,7 +2370,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>198</v>
       </c>
@@ -2391,7 +2390,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>200</v>
       </c>
@@ -2411,7 +2410,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>202</v>
       </c>
@@ -2431,7 +2430,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>204</v>
       </c>
@@ -2451,7 +2450,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>206</v>
       </c>
@@ -2471,7 +2470,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>208</v>
       </c>
@@ -2491,7 +2490,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>210</v>
       </c>
@@ -2511,7 +2510,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>212</v>
       </c>
@@ -2531,7 +2530,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>214</v>
       </c>
@@ -2551,7 +2550,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>216</v>
       </c>
@@ -2571,7 +2570,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>218</v>
       </c>
@@ -2591,7 +2590,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>220</v>
       </c>
@@ -2611,7 +2610,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>222</v>
       </c>
@@ -2631,7 +2630,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>224</v>
       </c>
@@ -2651,7 +2650,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>226</v>
       </c>
@@ -2671,7 +2670,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>228</v>
       </c>
@@ -2691,7 +2690,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>230</v>
       </c>
@@ -2711,7 +2710,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>232</v>
       </c>
@@ -2731,7 +2730,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>234</v>
       </c>
@@ -2751,7 +2750,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>236</v>
       </c>
@@ -2771,7 +2770,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>238</v>
       </c>
@@ -2791,7 +2790,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>240</v>
       </c>
@@ -2811,7 +2810,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>242</v>
       </c>
@@ -2831,7 +2830,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>244</v>
       </c>
@@ -2851,7 +2850,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>246</v>
       </c>
@@ -2871,7 +2870,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>248</v>
       </c>
@@ -2891,7 +2890,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>250</v>
       </c>
@@ -2911,7 +2910,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>252</v>
       </c>
@@ -2931,7 +2930,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>254</v>
       </c>
@@ -2951,7 +2950,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>256</v>
       </c>
@@ -2971,7 +2970,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>258</v>
       </c>
@@ -2991,7 +2990,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>260</v>
       </c>
@@ -3011,7 +3010,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>262</v>
       </c>
@@ -3031,7 +3030,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>264</v>
       </c>
@@ -3051,7 +3050,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>266</v>
       </c>
@@ -3071,7 +3070,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>268</v>
       </c>
@@ -3091,7 +3090,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>270</v>
       </c>
@@ -3111,7 +3110,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>272</v>
       </c>
@@ -3131,7 +3130,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>274</v>
       </c>
@@ -3151,7 +3150,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>276</v>
       </c>
@@ -3171,7 +3170,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>278</v>
       </c>
@@ -3191,7 +3190,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>280</v>
       </c>
@@ -3211,7 +3210,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>282</v>
       </c>
@@ -3231,7 +3230,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>284</v>
       </c>
@@ -3251,7 +3250,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>286</v>
       </c>
@@ -3271,7 +3270,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>288</v>
       </c>
@@ -3291,7 +3290,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>290</v>
       </c>
@@ -3311,7 +3310,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>292</v>
       </c>
@@ -3331,7 +3330,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>294</v>
       </c>
@@ -3351,7 +3350,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>296</v>
       </c>
@@ -3371,7 +3370,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>298</v>
       </c>
@@ -3391,7 +3390,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>300</v>
       </c>
@@ -3411,7 +3410,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>302</v>
       </c>

</xml_diff>